<commit_message>
Initial Commit - Alpha Project
</commit_message>
<xml_diff>
--- a/aws/alpha-project/src/aws-etl-alpha.xlsx
+++ b/aws/alpha-project/src/aws-etl-alpha.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\EDW\konigio\konig-examples\aws\alpha-project\src\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\EDW\konig-examples-test\aws\alpha-project\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -54,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="335" uniqueCount="232">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="333" uniqueCount="230">
   <si>
     <t>Class Name</t>
   </si>
@@ -726,12 +726,6 @@
     <t>t2.micro</t>
   </si>
   <si>
-    <t>D</t>
-  </si>
-  <si>
-    <t>$</t>
-  </si>
-  <si>
     <t>ECRRepositoryName</t>
   </si>
   <si>
@@ -750,7 +744,7 @@
     <t>alias</t>
   </si>
   <si>
-    <t xml:space="preserve">"AWSTemplateFormatVersion: '2010-09-09'
+    <t xml:space="preserve">AWSTemplateFormatVersion: '2010-09-09'
 Parameters:
   DesiredCapacity:
     Type: Number
@@ -955,6 +949,18 @@
               - 'ec2:Describe*'
               - 'ec2:AuthorizeSecurityGroupIngress'
             Resource: '*'
+  ECSTaskExecutionRole:
+    Type: 'AWS::IAM::Role'
+    Properties:
+      AssumeRolePolicyDocument:
+        Version: 2012-10-17
+        Statement:
+          - Effect: Allow
+            Principal:
+              Service: ecs-tasks.amazonaws.com
+            Action: ""sts:AssumeRole""
+      ManagedPolicyArns:
+        - 'arn:aws:iam::aws:policy/service-role/AmazonECSTaskExecutionRolePolicy'
   EC2Role:
     Type: AWS::IAM::Role
     Properties:
@@ -984,18 +990,6 @@
               - 'ecr:BatchGetImage'
               - 'ecr:GetDownloadUrlForLayer'
             Resource: '*'
-  ECSTaskExecutionRole:
-    Type: 'AWS::IAM::Role'
-    Properties:
-      AssumeRolePolicyDocument:
-        Version: 2012-10-17
-        Statement:
-          - Effect: Allow
-            Principal:
-              Service: ecs-tasks.amazonaws.com
-            Action: "sts:AssumeRole"
-      ManagedPolicyArns:
-        - 'arn:aws:iam::aws:policy/service-role/AmazonECSTaskExecutionRolePolicy'
   AutoscalingRole:
     Type: AWS::IAM::Role
     Properties:
@@ -1033,7 +1027,7 @@
     Description: The name of the ECS cluster, used by the deploy script
     Value: !Ref 'ECSCluster'
     Export:
-      Name: !Join [':', [!Ref ""AWS::StackName"", ""ClusterName"" ]]
+      Name: !Join [':', [!Ref "AWS::StackName", "ClusterName" ]]
   Url:
     Description: The url at which the application is available
     Value: !Join ['', [!GetAtt 'ECSALB.DNSName']]
@@ -1041,18 +1035,17 @@
     Description: The ARN of the ALB, exported for later use in creating services
     Value: !Ref 'ECSALB'
     Export:
-      Name: !Join [':', [!Ref ""AWS::StackName"", ""ALBArn"" ]]
+      Name: !Join [':', [!Ref "AWS::StackName", "ALBArn" ]]
   ECSRole:
     Description: The ARN of the ECS role, exports for later use in creating services
     Value: !GetAtt 'ECSServiceRole.Arn'
     Export:
-      Name: !Join [':', [!Ref ""AWS::StackName"", ""ECSRole"" ]]
+      Name: !Join [':', [!Ref "AWS::StackName", "ECSRole" ]]
   VPCId:
     Description: The ID of the VPC that this stack is deployed in
     Value: !Ref 'VPC'
     Export:
-      Name: !Join [':', [!Ref ""AWS::StackName"", ""VPCId"" ]]
-"
+      Name: !Join [':', [!Ref "AWS::StackName", "VPCId" ]]
 </t>
   </si>
 </sst>
@@ -1720,6 +1713,54 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>556260</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>91440</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="6" name="AutoShape 2"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="7620000" cy="7620000"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -2207,16 +2248,16 @@
     </row>
     <row r="11" spans="1:14" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="54" t="s">
+        <v>225</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>226</v>
+      </c>
+      <c r="C11" s="55" t="s">
         <v>227</v>
       </c>
-      <c r="B11" s="5" t="s">
+      <c r="D11" s="54" t="s">
         <v>228</v>
-      </c>
-      <c r="C11" s="55" t="s">
-        <v>229</v>
-      </c>
-      <c r="D11" s="54" t="s">
-        <v>230</v>
       </c>
       <c r="E11" s="21"/>
       <c r="F11" s="21"/>
@@ -12936,10 +12977,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B999"/>
+  <dimension ref="A1:B998"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="N20" sqref="N20"/>
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -12998,14 +13039,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="53" t="s">
-        <v>225</v>
-      </c>
-      <c r="B7" s="37" t="s">
-        <v>226</v>
-      </c>
-    </row>
+    <row r="7" spans="1:2" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="8" spans="1:2" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="9" spans="1:2" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="10" spans="1:2" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -13997,7 +14031,6 @@
     <row r="996" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="997" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="998" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="999" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -14009,7 +14042,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H17" sqref="H2:H17"/>
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -14031,7 +14064,7 @@
         <v>190</v>
       </c>
       <c r="B2" s="56" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated cloudfomation template and security tags
</commit_message>
<xml_diff>
--- a/aws/alpha-project/src/aws-etl-alpha.xlsx
+++ b/aws/alpha-project/src/aws-etl-alpha.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\EDW\konig-examples-test\aws\alpha-project\src\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\598182\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9192" firstSheet="1" activeTab="7"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9192" firstSheet="4" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="Ontologies" sheetId="1" r:id="rId1"/>
@@ -19,14 +19,15 @@
     <sheet name="Shapes" sheetId="5" r:id="rId5"/>
     <sheet name="Property Constraints" sheetId="6" r:id="rId6"/>
     <sheet name="Settings" sheetId="9" r:id="rId7"/>
-    <sheet name="Cloud Formation Templates" sheetId="7" r:id="rId8"/>
-    <sheet name="AmazonRDSCluster" sheetId="8" r:id="rId9"/>
+    <sheet name="AmazonRDSCluster" sheetId="8" r:id="rId8"/>
+    <sheet name="Cloud Formation Templates" sheetId="7" r:id="rId9"/>
+    <sheet name="Security Tags" sheetId="10" r:id="rId10"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Properties!$A$1:$H$47</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">'Property Constraints'!$A$1:$K$16</definedName>
   </definedNames>
-  <calcPr calcId="0"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
@@ -54,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="333" uniqueCount="230">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="373" uniqueCount="255">
   <si>
     <t>Class Name</t>
   </si>
@@ -744,223 +745,353 @@
     <t>alias</t>
   </si>
   <si>
-    <t xml:space="preserve">AWSTemplateFormatVersion: '2010-09-09'
+    <r>
+      <t>AWS Region</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+  </si>
+  <si>
+    <t>Amazon Resource Name</t>
+  </si>
+  <si>
+    <t>Tag Key</t>
+  </si>
+  <si>
+    <t>Tag Value</t>
+  </si>
+  <si>
+    <t>Environment</t>
+  </si>
+  <si>
+    <t>t_cost_centre</t>
+  </si>
+  <si>
+    <t>Development</t>
+  </si>
+  <si>
+    <t>t_name</t>
+  </si>
+  <si>
+    <t>t_owner_individual</t>
+  </si>
+  <si>
+    <t>t_responsible_individuals</t>
+  </si>
+  <si>
+    <t>t_environment</t>
+  </si>
+  <si>
+    <t>t_awscon</t>
+  </si>
+  <si>
+    <t>t_role</t>
+  </si>
+  <si>
+    <t>t_AppID</t>
+  </si>
+  <si>
+    <t>t_shut</t>
+  </si>
+  <si>
+    <t>t_pillar</t>
+  </si>
+  <si>
+    <t>t_cmdb</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>Foundation</t>
+  </si>
+  <si>
+    <t>t_dcl</t>
+  </si>
+  <si>
+    <t>DCL3</t>
+  </si>
+  <si>
+    <t>Vikram Medishetty</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AWSTemplateFormatVersion: 2010-09-09
+Description: &gt;-
+  A stack for deploying containerized applications in AWS Fargate. This stack
+  runs containers in a public VPC subnet, and includes a public facing load
+  balancer to register the services in.
 Parameters:
-  DesiredCapacity:
+  StackName:
+    Type: String
+    Default: test-edw-core
+    Description: &gt;-
+      The name of the parent Fargate networking stack that you created.
+      Necessary to locate and reference resources created by that stack.
+  ServiceName:
+    Type: String
+    Default: nginx
+    Description: A name for the service
+  Path:
+    Type: String
+    Default: '*'
+    Description: &gt;-
+      A path on the public load balancer that this service should be connected
+      to. Use * to send all load balancer traffic to this service.
+  DesiredCount:
     Type: Number
-    Default: '2'
-    Description: Number of instances to launch in your ECS cluster.
-  MaxSize:
+    Default: 1
+    Description: How many copies of the service task to run
+  ContainerPort:
     Type: Number
-    Default: '2'
-    Description: Maximum number of instances that can be launched in your ECS cluster.
-  InstanceType:
-    Description: EC2 instance type
+    Default: 80
+    Description: What port number the application inside the docker container is binding to
+  ContainerCpu:
+    Type: Number
+    Default: 512
+    Description: How much CPU to give the container. 1024 is 1 CPU
+  ContainerMemory:
+    Type: Number
+    Default: 1024
+    Description: How much memory in megabytes to give the container
+  Role:
     Type: String
-    Default: ${instanceTypeDefault}
-    AllowedValues: [t2.micro, t2.small, t2.medium, t2.large, m3.medium, m3.large,
-      m3.xlarge, m3.2xlarge, m4.large, m4.xlarge, m4.2xlarge, m4.4xlarge, m4.10xlarge,
-      c4.large, c4.xlarge, c4.2xlarge, c4.4xlarge, c4.8xlarge, c3.large, c3.xlarge,
-      c3.2xlarge, c3.4xlarge, c3.8xlarge, r3.large, r3.xlarge, r3.2xlarge, r3.4xlarge,
-      r3.8xlarge, i2.xlarge, i2.2xlarge, i2.4xlarge, i2.8xlarge]
-    ConstraintDescription: Please choose a valid instance type.
+    Default: ''
+    Description: &gt;-
+      (Optional) An IAM role to give the service's containers if the code within
+      needs to access other AWS resources like S3 buckets, DynamoDB tables, etc
 Mappings:
-  AWSRegionToAMI:
-    us-east-1:
-      AMIID: ami-eca289fb
-    us-east-2:
-      AMIID: ami-446f3521
-    us-west-1:
-      AMIID: ami-9fadf8ff
-    us-west-2:
-      AMIID: ami-7abc111a
-    eu-west-1:
-      AMIID: ami-a1491ad2
-    eu-central-1:
-      AMIID: ami-54f5303b
-    ap-northeast-1:
-      AMIID: ami-9cd57ffd
-    ap-southeast-1:
-      AMIID: ami-a900a3ca
-    ap-southeast-2:
-      AMIID: ami-5781be34
   SubnetConfig:
     VPC:
-      CIDR: '10.0.0.0/16'
+      CIDR: 10.0.0.0/16
     PublicOne:
-      CIDR: '10.0.0.0/24'
+      CIDR: 10.0.0.0/24
     PublicTwo:
-      CIDR: '10.0.1.0/24'
+      CIDR: 10.0.1.0/24
 Resources:
-  # VPC into which stack instances will be placed
   VPC:
-    Type: AWS::EC2::VPC
+    Type: 'AWS::EC2::VPC'
     Properties:
       EnableDnsSupport: true
       EnableDnsHostnames: true
-      CidrBlock: !FindInMap ['SubnetConfig', 'VPC', 'CIDR']
+      CidrBlock: !FindInMap 
+        - SubnetConfig
+        - VPC
+        - CIDR
+      Tags:
+      - Key: Name
+        Value: !Join 
+        - ''
+        - - !Ref 'AWS::StackName'
+          - ' resource'
+      $functions.mergeSecurityTags("VPC")
   PublicSubnetOne:
-    Type: AWS::EC2::Subnet
+    Type: 'AWS::EC2::Subnet'
     Properties:
-      AvailabilityZone:
-         Fn::Select:
-         - 0
-         - Fn::GetAZs: {Ref: 'AWS::Region'}
-      VpcId: !Ref 'VPC'
-      CidrBlock: !FindInMap ['SubnetConfig', 'PublicOne', 'CIDR']
+      AvailabilityZone: !Select 
+        - 0
+        - !GetAZs 
+          Ref: 'AWS::Region'
+      VpcId: !Ref VPC
+      CidrBlock: !FindInMap 
+        - SubnetConfig
+        - PublicOne
+        - CIDR
       MapPublicIpOnLaunch: true
+      Tags:
+      $functions.mergeSecurityTags("PublicSubnetOne")
   PublicSubnetTwo:
-    Type: AWS::EC2::Subnet
+    Type: 'AWS::EC2::Subnet'
     Properties:
-      AvailabilityZone:
-         Fn::Select:
-         - 1
-         - Fn::GetAZs: {Ref: 'AWS::Region'}
-      VpcId: !Ref 'VPC'
-      CidrBlock: !FindInMap ['SubnetConfig', 'PublicTwo', 'CIDR']
+      AvailabilityZone: !Select 
+        - 1
+        - !GetAZs 
+          Ref: 'AWS::Region'
+      VpcId: !Ref VPC
+      CidrBlock: !FindInMap 
+        - SubnetConfig
+        - PublicTwo
+        - CIDR
       MapPublicIpOnLaunch: true
   InternetGateway:
-    Type: AWS::EC2::InternetGateway
+    Type: 'AWS::EC2::InternetGateway'
   GatewayAttachement:
-    Type: AWS::EC2::VPCGatewayAttachment
+    Type: 'AWS::EC2::VPCGatewayAttachment'
     Properties:
-      VpcId: !Ref 'VPC'
-      InternetGatewayId: !Ref 'InternetGateway'
+      VpcId: !Ref VPC
+      InternetGatewayId: !Ref InternetGateway
   PublicRouteTable:
-    Type: AWS::EC2::RouteTable
+    Type: 'AWS::EC2::RouteTable'
     Properties:
-      VpcId: !Ref 'VPC'
+      VpcId: !Ref VPC
   PublicRoute:
-    Type: AWS::EC2::Route
+    Type: 'AWS::EC2::Route'
     DependsOn: GatewayAttachement
     Properties:
-      RouteTableId: !Ref 'PublicRouteTable'
-      DestinationCidrBlock: '0.0.0.0/0'
-      GatewayId: !Ref 'InternetGateway'
+      RouteTableId: !Ref PublicRouteTable
+      DestinationCidrBlock: 0.0.0.0/0
+      GatewayId: !Ref InternetGateway
   PublicSubnetOneRouteTableAssociation:
-    Type: AWS::EC2::SubnetRouteTableAssociation
+    Type: 'AWS::EC2::SubnetRouteTableAssociation'
     Properties:
       SubnetId: !Ref PublicSubnetOne
       RouteTableId: !Ref PublicRouteTable
   PublicSubnetTwoRouteTableAssociation:
-    Type: AWS::EC2::SubnetRouteTableAssociation
+    Type: 'AWS::EC2::SubnetRouteTableAssociation'
     Properties:
       SubnetId: !Ref PublicSubnetTwo
       RouteTableId: !Ref PublicRouteTable
-  # ECS Resources
   ECSCluster:
-    Type: AWS::ECS::Cluster
-  EcsSecurityGroup:
-    Type: AWS::EC2::SecurityGroup
+    Type: 'AWS::ECS::Cluster'
+  FargateContainerSecurityGroup:
+    Type: 'AWS::EC2::SecurityGroup'
     Properties:
-      GroupDescription: ECS Security Group
-      VpcId: !Ref 'VPC'
-  EcsSecurityGroupHTTPinbound:
-    Type: AWS::EC2::SecurityGroupIngress
+      GroupDescription: Access to the Fargate containers
+      VpcId: !Ref VPC
+  EcsSecurityGroupIngressFromPublicALB:
+    Type: 'AWS::EC2::SecurityGroupIngress'
     Properties:
-      GroupId: !Ref 'EcsSecurityGroup'
-      IpProtocol: tcp
-      FromPort: '80'
-      ToPort: '80'
-      CidrIp: 0.0.0.0/0
-  EcsSecurityGroupSSHinbound:
-    Type: AWS::EC2::SecurityGroupIngress
+      Description: Ingress from the public ALB
+      GroupId: !Ref FargateContainerSecurityGroup
+      IpProtocol: -1
+      SourceSecurityGroupId: !Ref PublicLoadBalancerSG
+  EcsSecurityGroupIngressFromSelf:
+    Type: 'AWS::EC2::SecurityGroupIngress'
     Properties:
-      GroupId: !Ref 'EcsSecurityGroup'
-      IpProtocol: tcp
-      FromPort: '22'
-      ToPort: '22'
-      CidrIp: 0.0.0.0/0
-  EcsSecurityGroupALBports:
-    Type: AWS::EC2::SecurityGroupIngress
+      Description: Ingress from other containers in the same security group
+      GroupId: !Ref FargateContainerSecurityGroup
+      IpProtocol: -1
+      SourceSecurityGroupId: !Ref FargateContainerSecurityGroup
+  PublicLoadBalancerSG:
+    Type: 'AWS::EC2::SecurityGroup'
     Properties:
-      GroupId: !Ref 'EcsSecurityGroup'
-      IpProtocol: tcp
-      FromPort: '31000'
-      ToPort: '61000'
-      SourceSecurityGroupId: !Ref 'EcsSecurityGroup'
-  CloudwatchLogsGroup:
-    Type: AWS::Logs::LogGroup
+      GroupDescription: Access to the public facing load balancer
+      VpcId: !Ref VPC
+      SecurityGroupIngress:
+        - CidrIp: 0.0.0.0/0
+          IpProtocol: -1
+  PublicLoadBalancer:
+    Type: 'AWS::ElasticLoadBalancingV2::LoadBalancer'
     Properties:
-      LogGroupName: !Join ['-', [ECSLogGroup, !Ref 'AWS::StackName']]
-      RetentionInDays: 14
-  ECSALB:
-    Type: AWS::ElasticLoadBalancingV2::LoadBalancer
-    Properties:
-      Name: demo
       Scheme: internet-facing
       LoadBalancerAttributes:
-      - Key: idle_timeout.timeout_seconds
-        Value: '30'
+        - Key: idle_timeout.timeout_seconds
+          Value: '30'
       Subnets:
         - !Ref PublicSubnetOne
         - !Ref PublicSubnetTwo
-      SecurityGroups: [!Ref 'EcsSecurityGroup']
-  ECSAutoScalingGroup:
-    Type: AWS::AutoScaling::AutoScalingGroup
+      SecurityGroups:
+        - !Ref PublicLoadBalancerSG
+  TargetGroupPublic:
+    Type: 'AWS::ElasticLoadBalancingV2::TargetGroup'
     Properties:
-      VPCZoneIdentifier:
-        - !Ref PublicSubnetOne
-        - !Ref PublicSubnetTwo
-      LaunchConfigurationName: !Ref 'ContainerInstances'
-      MinSize: '1'
-      MaxSize: !Ref 'MaxSize'
-      DesiredCapacity: !Ref 'DesiredCapacity'
-    CreationPolicy:
-      ResourceSignal:
-        Timeout: PT15M
-    UpdatePolicy:
-      AutoScalingReplacingUpdate:
-        WillReplace: 'true'
-  ContainerInstances:
-    Type: AWS::AutoScaling::LaunchConfiguration
+      HealthCheckIntervalSeconds: 70
+      HealthCheckPath: /health
+      HealthCheckProtocol: HTTP
+      HealthCheckTimeoutSeconds: 60
+      HealthyThresholdCount: 10
+      Port: 8080
+      Protocol: HTTP
+      UnhealthyThresholdCount: 10
+      VpcId: !Ref VPC
+  PublicLoadBalancerListener:
+    Type: 'AWS::ElasticLoadBalancingV2::Listener'
+    DependsOn:
+      - PublicLoadBalancer
     Properties:
-      ImageId: !FindInMap [AWSRegionToAMI, !Ref 'AWS::Region', AMIID]
-      SecurityGroups: [!Ref 'EcsSecurityGroup']
-      InstanceType: !Ref 'InstanceType'
-      IamInstanceProfile: !Ref 'EC2InstanceProfile'
-      UserData:
-        Fn::Base64: !Sub |
-          #!/bin/bash -xe
-          echo ECS_CLUSTER=${ECSCluster} &gt;&gt; /etc/ecs/ecs.config
-          yum install -y aws-cfn-bootstrap
-          /opt/aws/bin/cfn-signal -e $? --stack ${D}{AWS::StackName} --resource ECSAutoScalingGroup --region ${D}{AWS::Region}
-  ECSServiceRole:
-    Type: AWS::IAM::Role
+      DefaultActions:
+        - TargetGroupArn: !Ref TargetGroupPublic
+          Type: forward
+      LoadBalancerArn: !Ref PublicLoadBalancer
+      Port: 8080
+      Protocol: HTTP
+  ECSRole:
+    Type: 'AWS::IAM::Role'
     Properties:
       AssumeRolePolicyDocument:
         Statement:
-        - Effect: Allow
-          Principal:
-            Service: [ecs.amazonaws.com]
-          Action: ['sts:AssumeRole']
+          - Effect: Allow
+            Principal:
+              Service:
+                - ecs.amazonaws.com
+            Action:
+              - 'sts:AssumeRole'
       Path: /
       Policies:
-      - PolicyName: ecs-service
-        PolicyDocument:
-          Statement:
-          - Effect: Allow
-            Action:
-              - 'elasticloadbalancing:DeregisterInstancesFromLoadBalancer'
-              - 'elasticloadbalancing:DeregisterTargets'
-              - 'elasticloadbalancing:Describe*'
-              - 'elasticloadbalancing:RegisterInstancesWithLoadBalancer'
-              - 'elasticloadbalancing:RegisterTargets'
-              - 'ec2:Describe*'
-              - 'ec2:AuthorizeSecurityGroupIngress'
-            Resource: '*'
+        - PolicyName: ecs-service
+          PolicyDocument:
+            Statement:
+              - Effect: Allow
+                Action:
+                  - 'ec2:AttachNetworkInterface'
+                  - 'ec2:CreateNetworkInterface'
+                  - 'ec2:CreateNetworkInterfacePermission'
+                  - 'ec2:DeleteNetworkInterface'
+                  - 'ec2:DeleteNetworkInterfacePermission'
+                  - 'ec2:Describe*'
+                  - 'ec2:DetachNetworkInterface'
+                  - 'elasticloadbalancing:DeregisterInstancesFromLoadBalancer'
+                  - 'elasticloadbalancing:DeregisterTargets'
+                  - 'elasticloadbalancing:Describe*'
+                  - 'elasticloadbalancing:RegisterInstancesWithLoadBalancer'
+                  - 'elasticloadbalancing:RegisterTargets'
+                Resource: '*'
   ECSTaskExecutionRole:
     Type: 'AWS::IAM::Role'
     Properties:
       AssumeRolePolicyDocument:
-        Version: 2012-10-17
         Statement:
           - Effect: Allow
             Principal:
-              Service: ecs-tasks.amazonaws.com
-            Action: ""sts:AssumeRole""
-      ManagedPolicyArns:
-        - 'arn:aws:iam::aws:policy/service-role/AmazonECSTaskExecutionRolePolicy'
+              Service:
+                - ecs-tasks.amazonaws.com
+            Action:
+              - 'sts:AssumeRole'
+      Path: /
+      Policies:
+        - PolicyName: AmazonECSTaskExecutionRolePolicy
+          PolicyDocument:
+            Statement:
+              - Effect: Allow
+                Action:
+                  - 'ecr:GetAuthorizationToken'
+                  - 'ecr:BatchCheckLayerAvailability'
+                  - 'ecr:GetDownloadUrlForLayer'
+                  - 'ecr:BatchGetImage'
+                  - 'logs:CreateLogStream'
+                  - 'logs:PutLogEvents'
+                Resource: '*'
+  TargetGroup:
+    Type: 'AWS::ElasticLoadBalancingV2::TargetGroup'
+    Properties:
+      HealthCheckIntervalSeconds: 70
+      HealthCheckPath: /health
+      HealthCheckProtocol: HTTP
+      HealthCheckTimeoutSeconds: 60
+      HealthyThresholdCount: 10
+      TargetType: ip
+      Port: 8080
+      Protocol: HTTP
+      UnhealthyThresholdCount: 10
+      VpcId: !Ref VPC
+  LoadBalancerRule:
+    Type: 'AWS::ElasticLoadBalancingV2::ListenerRule'
+    Properties:
+      Actions:
+        - TargetGroupArn: !Ref TargetGroup
+          Type: forward
+      Conditions:
+        - Field: path-pattern
+          Values:
+            - !Ref Path
+      ListenerArn: !Ref PublicLoadBalancerListener
+      Priority: 1  
   EC2Role:
     Type: AWS::IAM::Role
     Properties:
@@ -990,28 +1121,6 @@
               - 'ecr:BatchGetImage'
               - 'ecr:GetDownloadUrlForLayer'
             Resource: '*'
-  AutoscalingRole:
-    Type: AWS::IAM::Role
-    Properties:
-      AssumeRolePolicyDocument:
-        Statement:
-        - Effect: Allow
-          Principal:
-            Service: [application-autoscaling.amazonaws.com]
-          Action: ['sts:AssumeRole']
-      Path: /
-      Policies:
-      - PolicyName: service-autoscaling
-        PolicyDocument:
-          Statement:
-          - Effect: Allow
-            Action:
-              - 'application-autoscaling:*'
-              - 'cloudwatch:DescribeAlarms'
-              - 'cloudwatch:PutMetricAlarm'
-              - 'ecs:DescribeServices'
-              - 'ecs:UpdateService'
-            Resource: '*'
   EC2InstanceProfile:
     Type: AWS::IAM::InstanceProfile
     Properties:
@@ -1022,6 +1131,10 @@
     Properties:
       Path: /
       Roles: [!Ref 'ECSTaskExecutionRole']
+  CloudwatchLogsGroup:
+    Type: AWS::Logs::LogGroup
+    Properties:
+      LogGroupName: !Ref 'AWS::StackName'
 Outputs:
   ClusterName:
     Description: The name of the ECS cluster, used by the deploy script
@@ -1030,17 +1143,7 @@
       Name: !Join [':', [!Ref "AWS::StackName", "ClusterName" ]]
   Url:
     Description: The url at which the application is available
-    Value: !Join ['', [!GetAtt 'ECSALB.DNSName']]
-  ALBArn:
-    Description: The ARN of the ALB, exported for later use in creating services
-    Value: !Ref 'ECSALB'
-    Export:
-      Name: !Join [':', [!Ref "AWS::StackName", "ALBArn" ]]
-  ECSRole:
-    Description: The ARN of the ECS role, exports for later use in creating services
-    Value: !GetAtt 'ECSServiceRole.Arn'
-    Export:
-      Name: !Join [':', [!Ref "AWS::StackName", "ECSRole" ]]
+    Value: !Join ['', [!GetAtt 'PublicLoadBalancer.DNSName']]
   VPCId:
     Description: The ID of the VPC that this stack is deployed in
     Value: !Ref 'VPC'
@@ -1048,12 +1151,21 @@
       Name: !Join [':', [!Ref "AWS::StackName", "VPCId" ]]
 </t>
   </si>
+  <si>
+    <t>Sofaops@pearson.com</t>
+  </si>
+  <si>
+    <t>edw_core</t>
+  </si>
+  <si>
+    <t>edw_core_role</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="19" x14ac:knownFonts="1">
+  <fonts count="23" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -1148,6 +1260,30 @@
       <u/>
       <sz val="10"/>
       <color rgb="FF000000"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="10"/>
       <name val="Arial"/>
     </font>
   </fonts>
@@ -1272,10 +1408,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="57">
+  <cellXfs count="60">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1379,8 +1516,12 @@
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="20" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="7">
@@ -1729,6 +1870,1878 @@
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
         <xdr:cNvPr id="6" name="AutoShape 2"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="7620000" cy="7620000"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>556260</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>91440</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="7" name="AutoShape 2"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="7620000" cy="7620000"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>556260</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>91440</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="8" name="AutoShape 2"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="7620000" cy="7620000"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>556260</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>91440</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="9" name="AutoShape 2"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="7620000" cy="7620000"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>556260</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>91440</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="10" name="AutoShape 2"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="7620000" cy="7620000"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>556260</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>91440</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="11" name="AutoShape 2"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="7620000" cy="7620000"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>556260</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>91440</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="12" name="AutoShape 2"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="7620000" cy="7620000"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>556260</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>91440</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="13" name="AutoShape 2"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="7620000" cy="7620000"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>556260</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>91440</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="14" name="AutoShape 2"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="7620000" cy="7620000"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>556260</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>91440</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="15" name="AutoShape 2"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="7620000" cy="7620000"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>556260</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>91440</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="16" name="AutoShape 2"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="7620000" cy="7620000"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>556260</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>91440</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="17" name="AutoShape 2"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="7620000" cy="7620000"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>556260</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>91440</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="18" name="AutoShape 2"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="7620000" cy="7620000"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>556260</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>91440</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="19" name="AutoShape 2"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="7620000" cy="7620000"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>556260</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>91440</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="20" name="AutoShape 2"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="7620000" cy="7620000"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>556260</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>91440</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="21" name="AutoShape 2"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="7620000" cy="7620000"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>556260</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>91440</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="22" name="AutoShape 2"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="7620000" cy="7620000"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>556260</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>91440</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="23" name="AutoShape 2"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="7620000" cy="7620000"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>556260</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>91440</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="24" name="AutoShape 2"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="7620000" cy="7620000"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>556260</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>91440</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="25" name="AutoShape 2"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="7620000" cy="7620000"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>556260</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>91440</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="26" name="AutoShape 2"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="7620000" cy="7620000"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>556260</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>91440</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="27" name="AutoShape 2"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="7620000" cy="7620000"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>556260</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>91440</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="28" name="AutoShape 2"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="7620000" cy="7620000"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>556260</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>91440</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="29" name="AutoShape 2"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="7620000" cy="7620000"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>556260</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>91440</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="30" name="AutoShape 2"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="7620000" cy="7620000"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>556260</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>91440</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="31" name="AutoShape 2"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="7620000" cy="7620000"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>556260</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>91440</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="32" name="AutoShape 2"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="7620000" cy="7620000"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>556260</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>91440</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="33" name="AutoShape 2"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="7620000" cy="7620000"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>556260</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>91440</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="34" name="AutoShape 2"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="7620000" cy="7620000"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>556260</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>91440</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="35" name="AutoShape 2"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="7620000" cy="7620000"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>556260</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>91440</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="36" name="AutoShape 2"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="7620000" cy="7620000"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>556260</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>91440</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="37" name="AutoShape 2"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="7620000" cy="7620000"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>556260</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>91440</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="38" name="AutoShape 2"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="7620000" cy="7620000"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>556260</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>91440</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="39" name="AutoShape 2"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="7620000" cy="7620000"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>556260</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>91440</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="40" name="AutoShape 2"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="7620000" cy="7620000"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>556260</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>91440</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="41" name="AutoShape 2"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="7620000" cy="7620000"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>556260</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>91440</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="42" name="AutoShape 2"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="7620000" cy="7620000"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>556260</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>91440</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="43" name="AutoShape 2"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="7620000" cy="7620000"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>556260</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>91440</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="44" name="AutoShape 2"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="7620000" cy="7620000"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>556260</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>91440</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="45" name="AutoShape 2"/>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -3275,6 +5288,189 @@
   <printOptions horizontalCentered="1" gridLines="1"/>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup fitToHeight="0" pageOrder="overThenDown" orientation="landscape" cellComments="atEnd"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D13"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="54.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="55" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.88671875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" s="37" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="50" t="s">
+        <v>230</v>
+      </c>
+      <c r="B1" s="57" t="s">
+        <v>231</v>
+      </c>
+      <c r="C1" s="57" t="s">
+        <v>232</v>
+      </c>
+      <c r="D1" s="57" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A2" s="52"/>
+      <c r="B2" s="58" t="s">
+        <v>234</v>
+      </c>
+      <c r="C2" s="58">
+        <v>3651091</v>
+      </c>
+      <c r="D2" s="58" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A3" s="52"/>
+      <c r="B3" s="58" t="s">
+        <v>236</v>
+      </c>
+      <c r="C3" s="58" t="s">
+        <v>253</v>
+      </c>
+      <c r="D3" s="58" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A4" s="52"/>
+      <c r="B4" s="58" t="s">
+        <v>237</v>
+      </c>
+      <c r="C4" s="58" t="s">
+        <v>250</v>
+      </c>
+      <c r="D4" s="58" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A5" s="52"/>
+      <c r="B5" s="58" t="s">
+        <v>238</v>
+      </c>
+      <c r="C5" s="59" t="s">
+        <v>252</v>
+      </c>
+      <c r="D5" s="58" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A6" s="52"/>
+      <c r="B6" s="58" t="s">
+        <v>239</v>
+      </c>
+      <c r="C6" s="58" t="s">
+        <v>235</v>
+      </c>
+      <c r="D6" s="58" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A7" s="52"/>
+      <c r="B7" s="58" t="s">
+        <v>240</v>
+      </c>
+      <c r="C7" s="58" t="s">
+        <v>235</v>
+      </c>
+      <c r="D7" s="58" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A8" s="52"/>
+      <c r="B8" s="58" t="s">
+        <v>241</v>
+      </c>
+      <c r="C8" s="58" t="s">
+        <v>254</v>
+      </c>
+      <c r="D8" s="58" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A9" s="52"/>
+      <c r="B9" s="58" t="s">
+        <v>242</v>
+      </c>
+      <c r="C9" s="58">
+        <v>123</v>
+      </c>
+      <c r="D9" s="58" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A10" s="52"/>
+      <c r="B10" s="58" t="s">
+        <v>243</v>
+      </c>
+      <c r="C10" s="58" t="s">
+        <v>246</v>
+      </c>
+      <c r="D10" s="58" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A11" s="52"/>
+      <c r="B11" s="58" t="s">
+        <v>244</v>
+      </c>
+      <c r="C11" s="58" t="s">
+        <v>247</v>
+      </c>
+      <c r="D11" s="58" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A12" s="52"/>
+      <c r="B12" s="58" t="s">
+        <v>245</v>
+      </c>
+      <c r="C12" s="58" t="s">
+        <v>246</v>
+      </c>
+      <c r="D12" s="58" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A13" s="52"/>
+      <c r="B13" s="58" t="s">
+        <v>248</v>
+      </c>
+      <c r="C13" s="58" t="s">
+        <v>249</v>
+      </c>
+      <c r="D13" s="58" t="s">
+        <v>235</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C5" r:id="rId1"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -8822,8 +11018,8 @@
   </sheetPr>
   <dimension ref="A1:U1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -8873,7 +11069,7 @@
       <c r="K1" s="19" t="s">
         <v>110</v>
       </c>
-      <c r="L1" s="50" t="s">
+      <c r="L1" s="19" t="s">
         <v>187</v>
       </c>
       <c r="M1" s="21"/>
@@ -8900,15 +11096,13 @@
       <c r="E2" s="21" t="s">
         <v>112</v>
       </c>
-      <c r="F2" s="23"/>
+      <c r="F2" s="21"/>
       <c r="G2" s="23"/>
       <c r="H2" s="23"/>
       <c r="I2" s="23"/>
       <c r="J2" s="23"/>
       <c r="K2" s="27"/>
-      <c r="L2" s="21" t="s">
-        <v>130</v>
-      </c>
+      <c r="L2" s="21"/>
       <c r="M2" s="21"/>
       <c r="N2" s="21"/>
       <c r="O2" s="21"/>
@@ -8941,7 +11135,9 @@
       <c r="I3" s="23"/>
       <c r="J3" s="23"/>
       <c r="K3" s="27"/>
-      <c r="L3" s="21"/>
+      <c r="L3" s="21" t="s">
+        <v>111</v>
+      </c>
       <c r="M3" s="21"/>
       <c r="N3" s="21"/>
       <c r="O3" s="21"/>
@@ -10348,7 +12544,7 @@
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B9" sqref="B9"/>
+      <selection pane="bottomRight" activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -10517,7 +12713,7 @@
       <c r="A5" s="29" t="s">
         <v>111</v>
       </c>
-      <c r="B5" s="31" t="s">
+      <c r="B5" s="21" t="s">
         <v>37</v>
       </c>
       <c r="C5" s="40" t="s">
@@ -12980,7 +15176,7 @@
   <dimension ref="A1:B998"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+      <selection activeCell="J34" sqref="J34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -14039,46 +16235,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B2"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="13.6640625" style="37" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="24.109375" style="37" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="50" t="s">
-        <v>189</v>
-      </c>
-      <c r="B1" s="50" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="409.6" x14ac:dyDescent="0.25">
-      <c r="A2" s="37" t="s">
-        <v>190</v>
-      </c>
-      <c r="B2" s="56" t="s">
-        <v>229</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J9" sqref="J9"/>
+      <selection activeCell="E33" sqref="E33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -14174,4 +16334,47 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="13.6640625" style="37" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="134.44140625" style="37" customWidth="1"/>
+    <col min="3" max="3" width="11.5546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="15" x14ac:dyDescent="0.35">
+      <c r="A1" s="50" t="s">
+        <v>189</v>
+      </c>
+      <c r="B1" s="50" t="s">
+        <v>191</v>
+      </c>
+      <c r="C1" s="50" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="408.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="37" t="s">
+        <v>190</v>
+      </c>
+      <c r="B2" s="56" t="s">
+        <v>251</v>
+      </c>
+      <c r="C2" s="52" t="s">
+        <v>216</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>